<commit_message>
AFDP-5509: Send media stream and create job on AWS side - Configuration
</commit_message>
<xml_diff>
--- a/acm/rules/drools-transcribe-rules.xlsx
+++ b/acm/rules/drools-transcribe-rules.xlsx
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>language == null</t>
-  </si>
-  <si>
-    <t>setLanguage, 'en_US'</t>
   </si>
   <si>
     <t>RuleTable Transcribe Rules</t>
@@ -150,6 +147,9 @@
     return evaluated;
 }</t>
     </r>
+  </si>
+  <si>
+    <t>setLanguage, 'en-US'</t>
   </si>
 </sst>
 </file>
@@ -822,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -842,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -852,7 +852,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -942,7 +942,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -959,7 +959,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -1038,7 +1038,7 @@
         <v>29</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>